<commit_message>
implemented CR, CP, F, AR metrics and generated consolidated report
</commit_message>
<xml_diff>
--- a/category/cabin_baggage/results/answer_relevancy/summary/answer_relevancy_summary.xlsx
+++ b/category/cabin_baggage/results/answer_relevancy/summary/answer_relevancy_summary.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +481,11 @@
           <t>na_questions</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>execution_time_seconds</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -516,6 +521,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -551,6 +557,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -586,6 +593,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -621,6 +629,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -656,6 +665,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -691,6 +701,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="J7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -726,6 +737,7 @@
           <t>D</t>
         </is>
       </c>
+      <c r="J8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -761,6 +773,7 @@
           <t>-</t>
         </is>
       </c>
+      <c r="J9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -796,33 +809,75 @@
           <t>-</t>
         </is>
       </c>
+      <c r="J10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>35</v>
+      </c>
+      <c r="C11" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>85.7%</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0.6438</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Q, R, S, Q28, Q29</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>141.94</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
         <is>
           <t>TOTALS</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>9 runs</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="n">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10 runs</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
         <v>1</v>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>75.6%</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>0.5790999999999999</v>
-      </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>76.6%</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>0.5856</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
+        <v>141.94</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -892,10 +947,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -921,10 +976,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
@@ -934,7 +989,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>22.2%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -950,10 +1005,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -979,10 +1034,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
         <v>6</v>
@@ -992,7 +1047,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>66.7%</t>
+          <t>60.0%</t>
         </is>
       </c>
     </row>
@@ -1008,10 +1063,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
@@ -1021,7 +1076,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>22.2%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -1037,10 +1092,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" t="n">
         <v>2</v>
@@ -1050,7 +1105,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>22.2%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -1066,10 +1121,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
@@ -1095,10 +1150,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -1124,10 +1179,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1153,10 +1208,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11" t="n">
         <v>5</v>
@@ -1166,7 +1221,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>55.6%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -1182,10 +1237,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D12" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -1211,10 +1266,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" t="n">
         <v>2</v>
@@ -1224,7 +1279,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>22.2%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -1240,10 +1295,10 @@
         </is>
       </c>
       <c r="C14" t="n">
+        <v>10</v>
+      </c>
+      <c r="D14" t="n">
         <v>9</v>
-      </c>
-      <c r="D14" t="n">
-        <v>8</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
@@ -1253,7 +1308,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>10.0%</t>
         </is>
       </c>
     </row>
@@ -1269,10 +1324,10 @@
         </is>
       </c>
       <c r="C15" t="n">
+        <v>10</v>
+      </c>
+      <c r="D15" t="n">
         <v>9</v>
-      </c>
-      <c r="D15" t="n">
-        <v>8</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
@@ -1282,7 +1337,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>10.0%</t>
         </is>
       </c>
     </row>
@@ -1298,10 +1353,10 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1327,10 +1382,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D17" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1356,20 +1411,20 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D18" t="n">
         <v>5</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>44.4%</t>
+          <t>50.0%</t>
         </is>
       </c>
     </row>
@@ -1385,13 +1440,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -1414,13 +1469,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1443,10 +1498,10 @@
         </is>
       </c>
       <c r="C21" t="n">
+        <v>10</v>
+      </c>
+      <c r="D21" t="n">
         <v>9</v>
-      </c>
-      <c r="D21" t="n">
-        <v>8</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
@@ -1456,7 +1511,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>10.0%</t>
         </is>
       </c>
     </row>
@@ -1472,10 +1527,10 @@
         </is>
       </c>
       <c r="C22" t="n">
+        <v>10</v>
+      </c>
+      <c r="D22" t="n">
         <v>9</v>
-      </c>
-      <c r="D22" t="n">
-        <v>8</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
@@ -1485,7 +1540,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>10.0%</t>
         </is>
       </c>
     </row>
@@ -1501,10 +1556,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D23" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E23" t="n">
         <v>2</v>
@@ -1514,7 +1569,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>22.2%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -1530,10 +1585,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D24" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E24" t="n">
         <v>2</v>
@@ -1543,7 +1598,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>22.2%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -1559,10 +1614,10 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D25" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E25" t="n">
         <v>2</v>
@@ -1572,7 +1627,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>22.2%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -1588,10 +1643,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D26" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E26" t="n">
         <v>2</v>
@@ -1601,7 +1656,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>22.2%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -1617,10 +1672,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D27" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E27" t="n">
         <v>2</v>
@@ -1630,7 +1685,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>22.2%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -1646,10 +1701,10 @@
         </is>
       </c>
       <c r="C28" t="n">
+        <v>10</v>
+      </c>
+      <c r="D28" t="n">
         <v>9</v>
-      </c>
-      <c r="D28" t="n">
-        <v>8</v>
       </c>
       <c r="E28" t="n">
         <v>1</v>
@@ -1659,7 +1714,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>10.0%</t>
         </is>
       </c>
     </row>
@@ -1675,20 +1730,20 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D29" t="n">
         <v>8</v>
       </c>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -1704,13 +1759,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1733,10 +1788,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D31" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
@@ -1762,10 +1817,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D32" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
@@ -1791,10 +1846,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D33" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -1820,10 +1875,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D34" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E34" t="n">
         <v>4</v>
@@ -1833,7 +1888,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>44.4%</t>
+          <t>40.0%</t>
         </is>
       </c>
     </row>
@@ -1849,10 +1904,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D35" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E35" t="n">
         <v>2</v>
@@ -1862,7 +1917,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>22.2%</t>
+          <t>20.0%</t>
         </is>
       </c>
     </row>
@@ -1878,10 +1933,10 @@
         </is>
       </c>
       <c r="C36" t="n">
+        <v>10</v>
+      </c>
+      <c r="D36" t="n">
         <v>9</v>
-      </c>
-      <c r="D36" t="n">
-        <v>8</v>
       </c>
       <c r="E36" t="n">
         <v>1</v>
@@ -1891,7 +1946,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>11.1%</t>
+          <t>10.0%</t>
         </is>
       </c>
     </row>

</xml_diff>